<commit_message>
a few changes to things
</commit_message>
<xml_diff>
--- a/simulations.xlsx
+++ b/simulations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bangoroffice365-my.sharepoint.com/personal/tmg25bcx_bangor_ac_uk/Documents/Research/FESTIM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F25DC773A252ABDACC104835415B67785ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{165BBC58-00EC-4ADF-A4F3-43CBAD272988}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="11_F25DC773A252ABDACC104835415B67785ADE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45426AC8-AFCF-4529-B42E-701E2EE5AE77}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Simulation ID</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Machine</t>
   </si>
   <si>
-    <t>Software Version</t>
-  </si>
-  <si>
     <t>Input File</t>
   </si>
   <si>
@@ -63,82 +60,40 @@
     <t>SIM001</t>
   </si>
   <si>
-    <t>v1.4.2</t>
-  </si>
-  <si>
-    <t>input001.json</t>
-  </si>
-  <si>
-    <t>output001.csv</t>
-  </si>
-  <si>
-    <t>SIM002</t>
-  </si>
-  <si>
     <t>Windows (WSL)</t>
   </si>
   <si>
-    <t>input002.json</t>
-  </si>
-  <si>
-    <t>output002.csv</t>
-  </si>
-  <si>
-    <t>B increased</t>
-  </si>
-  <si>
-    <t>SIM003</t>
-  </si>
-  <si>
-    <t>v1.4.3-dev</t>
-  </si>
-  <si>
-    <t>input003.json</t>
-  </si>
-  <si>
-    <t>output003.csv</t>
-  </si>
-  <si>
-    <t>Crashed due to memory limit</t>
-  </si>
-  <si>
-    <t>SIM004</t>
-  </si>
-  <si>
-    <t>v1.4.3</t>
-  </si>
-  <si>
-    <t>input004.json</t>
-  </si>
-  <si>
-    <t>output004.csv</t>
-  </si>
-  <si>
-    <t>Testing new param set</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Complete</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Running</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
     <t>HPC</t>
   </si>
   <si>
-    <t>Locally</t>
-  </si>
-  <si>
-    <t>LiO2 Single Crystal</t>
+    <t>Param A Range</t>
+  </si>
+  <si>
+    <t>Param B Range</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>example.yamyl</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>300-400K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generation rate </t>
+  </si>
+  <si>
+    <t>thermal conductivity</t>
+  </si>
+  <si>
+    <t>tconc.txt</t>
   </si>
 </sst>
 </file>
@@ -484,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,12 +451,14 @@
     <col min="2" max="2" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.88671875" style="5" customWidth="1"/>
     <col min="4" max="4" width="11.44140625" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12.77734375" customWidth="1"/>
-    <col min="12" max="12" width="17.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -509,7 +466,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -521,175 +478,115 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B2" s="4">
         <v>45856</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="I2" s="2">
-        <v>100</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>37</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4">
-        <v>45856</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>100</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>19</v>
-      </c>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4">
-        <v>45857</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>200</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>24</v>
-      </c>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="4">
-        <v>45858</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="2">
-        <v>2</v>
-      </c>
-      <c r="H5" s="2">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2">
-        <v>100</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>29</v>
-      </c>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>